<commit_message>
- CHG: Aligned METADATA sheets.
- FIX: Fixed references to wrong templates.
</commit_message>
<xml_diff>
--- a/chemical-compound-data/compound-data.xlsx
+++ b/chemical-compound-data/compound-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\web-intellij\germinate\datatemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sr41756\workspaces\misc\germinate-data-templates\chemical-compound-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031DAD14-EABF-4E20-81BE-3DC6B2831469}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B2A08F-34CB-4F37-B3FA-CB8D3BEE3603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="3" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>CACTUAR-3</t>
   </si>
   <si>
-    <t>The "PHENOTYPES" sheet should contain a definition of the different phenotypic traits evaluated in your experiment. The "DATA" sheet should contain the phenotype values in a matrix format where the columns are the phenotype names and the rows are lines/germplasm names (ACCENUMB of the MCPD). Each cell should contain the phenotype value for the combination of phenotype and line/germplasm. Missing data should be represented by an empty cell (not NA or a dash). See the "DATA_EXAMPLE " sheet for an example. Also note, that we only deal with means, i.e. for each line/germplasm and phenotype there should only be one value. Replicates can be submitted across years by entereing them as different phenotype datasets. For example 'Phenotype Experiment 2016' and 'Phenotype Experiment 2017'.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">If you have any queries or want to discuss your data or require assistance in filling in this template please contact us on </t>
     </r>
@@ -247,6 +244,9 @@
   </si>
   <si>
     <t>Epicatechin</t>
+  </si>
+  <si>
+    <t>The "COMPOUNDS" sheet should contain a definition of the different chemical compounds evaluated in your experiment. The "DATA" sheet should contain the compound values in a matrix format where the columns are the compound names and the rows are lines/germplasm names (ACCENUMB of the MCPD). Each cell should contain the compound value for the combination of compound and line/germplasm. Missing data should be represented by an empty cell (not NA or a dash). See the "DATA_EXAMPLE " sheet for an example. Also note, that we only deal with means, i.e. for each line/germplasm and compound there should only be one value. Replicates can be submitted across years by entereing them as different compound datasets. For example 'Compound Experiment 2016' and 'Compound Experiment 2017'.</t>
   </si>
 </sst>
 </file>
@@ -437,6 +437,24 @@
   </cellStyles>
   <dxfs count="25">
     <dxf>
+      <numFmt numFmtId="164" formatCode="yyyymmdd"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyymmdd"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyymmdd"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
@@ -449,31 +467,6 @@
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="yyyymmdd"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="yyyymmdd"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="yyyymmdd"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -597,6 +590,13 @@
       </font>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -637,12 +637,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CDFAA9A6-0123-422D-B80F-81EB2270DAA0}" name="Table7" displayName="Table7" ref="A1:C12" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CDFAA9A6-0123-422D-B80F-81EB2270DAA0}" name="Table7" displayName="Table7" ref="A1:C12" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:C12" xr:uid="{DCA4608A-E2D9-45F1-81E3-F49396F38526}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1E03C996-7263-422B-8AA0-13669C78161F}" name="LABEL" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{A20F043F-90CD-41BB-866B-522B95F3EC18}" name="DEFINITION" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{139364FF-5D24-40BF-A84C-CF209A3E5D65}" name="VALUE" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{1E03C996-7263-422B-8AA0-13669C78161F}" name="LABEL" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{A20F043F-90CD-41BB-866B-522B95F3EC18}" name="DEFINITION" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{139364FF-5D24-40BF-A84C-CF209A3E5D65}" name="VALUE" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -664,16 +664,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35BDF020-ABCA-4439-B958-8014090B32CC}" name="Table8" displayName="Table8" ref="A1:G2" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35BDF020-ABCA-4439-B958-8014090B32CC}" name="Table8" displayName="Table8" ref="A1:G2" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:G2" xr:uid="{1B38FBA2-DC2A-4EE8-9782-869C402F129F}"/>
   <tableColumns count="7">
-    <tableColumn id="2" xr3:uid="{11A585B5-EAF2-4086-9D85-0D60A53887C4}" name="Last Name" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{4077ACA3-84ED-4981-AB4E-365AEBA76825}" name="First Name" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{0A90BD52-57A6-4CDE-BA8E-5136E8A1EAB8}" name="Email" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{03F1C9C1-7B2C-4F0C-B099-1F465D301B93}" name="Phone" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{65BCBC93-FC74-4E14-B6A5-BF465AB5D91D}" name="Contributor" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{5C332E95-780E-414E-B1E2-86318BE35F31}" name="Address" dataDxfId="10"/>
-    <tableColumn id="1" xr3:uid="{9A8DCFA6-0AF2-4BA7-95EB-E0D0FE3A6153}" name="Country" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{11A585B5-EAF2-4086-9D85-0D60A53887C4}" name="Last Name" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{4077ACA3-84ED-4981-AB4E-365AEBA76825}" name="First Name" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{0A90BD52-57A6-4CDE-BA8E-5136E8A1EAB8}" name="Email" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{03F1C9C1-7B2C-4F0C-B099-1F465D301B93}" name="Phone" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{65BCBC93-FC74-4E14-B6A5-BF465AB5D91D}" name="Contributor" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{5C332E95-780E-414E-B1E2-86318BE35F31}" name="Address" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{9A8DCFA6-0AF2-4BA7-95EB-E0D0FE3A6153}" name="Country" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -740,9 +740,9 @@
   <autoFilter ref="A1:D12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Line/Phenotype"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Quercetin" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Catechin" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Epicatechin" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Quercetin" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Catechin" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Epicatechin" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -753,9 +753,9 @@
   <autoFilter ref="A1:D12" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Line/Phenotype"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Quercetin" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Catechin" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Epicatechin" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Quercetin" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Catechin" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Epicatechin" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1026,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,21 +1043,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="C1" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="8"/>
     </row>
@@ -1066,79 +1066,79 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="19"/>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="8"/>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="C11" s="8"/>
     </row>
@@ -1147,7 +1147,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="5"/>
     </row>
@@ -1164,7 +1164,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1191,12 +1191,12 @@
         <v>11</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="22" priority="1">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1231,19 +1231,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>54</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1280,48 +1280,48 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>39</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>40</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>43</v>
-      </c>
       <c r="G1" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="C2" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="F2" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="20" t="s">
-        <v>49</v>
-      </c>
       <c r="G2" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1360,16 +1360,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>8</v>
@@ -1407,7 +1407,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="7" priority="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1431,7 +1431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6:F7"/>
     </sheetView>
   </sheetViews>
@@ -1442,7 +1442,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="6" priority="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1510,7 +1510,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -1559,16 +1559,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>8</v>
@@ -1582,11 +1582,11 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" s="3">
         <v>302.042664</v>
@@ -1595,7 +1595,7 @@
         <v>302.23599999999999</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -1603,10 +1603,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
         <v>65</v>
-      </c>
-      <c r="C3" t="s">
-        <v>66</v>
       </c>
       <c r="D3">
         <v>290.07904100000002</v>
@@ -1615,15 +1615,15 @@
         <v>290.26799999999997</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4">
         <v>290.07904100000002</v>
@@ -1632,7 +1632,7 @@
         <v>290.26799999999997</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1676,13 +1676,13 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1864,13 +1864,13 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- ADD: Added more metadata information.
- ADD: Added data point specific GPS information fields.

- CHG: Improved consistency between data templates.
</commit_message>
<xml_diff>
--- a/chemical-compound-data/compound-data.xlsx
+++ b/chemical-compound-data/compound-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sr41756\workspaces\misc\germinate-data-templates\chemical-compound-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B2A08F-34CB-4F37-B3FA-CB8D3BEE3603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22E486E-4E06-4536-A384-CFD441B7E2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -247,6 +247,54 @@
   </si>
   <si>
     <t>The "COMPOUNDS" sheet should contain a definition of the different chemical compounds evaluated in your experiment. The "DATA" sheet should contain the compound values in a matrix format where the columns are the compound names and the rows are lines/germplasm names (ACCENUMB of the MCPD). Each cell should contain the compound value for the combination of compound and line/germplasm. Missing data should be represented by an empty cell (not NA or a dash). See the "DATA_EXAMPLE " sheet for an example. Also note, that we only deal with means, i.e. for each line/germplasm and compound there should only be one value. Replicates can be submitted across years by entereing them as different compound datasets. For example 'Compound Experiment 2016' and 'Compound Experiment 2017'.</t>
+  </si>
+  <si>
+    <t>Investigation Title</t>
+  </si>
+  <si>
+    <t>Human-readable string summarising the investigation.</t>
+  </si>
+  <si>
+    <t>Investigation Description</t>
+  </si>
+  <si>
+    <t>Human-readable text describing the investigation in more detail.</t>
+  </si>
+  <si>
+    <t>Investigation unique ID</t>
+  </si>
+  <si>
+    <t>Identifier comprising the unique name of the institution/database hosting the submission of the investigation data, and the accession number of the investigation in that institution.</t>
+  </si>
+  <si>
+    <t>Associated data file link</t>
+  </si>
+  <si>
+    <t>Link to the data file (or digital object) in a public database or in a persistent institutional repository; or identifier of the data file when submitted together with the MIAPPE submission.</t>
+  </si>
+  <si>
+    <t>Associated data file description</t>
+  </si>
+  <si>
+    <t>Description of the format of the data file. May be a standard file format name, or a description of organization of the data in a tabular file.</t>
+  </si>
+  <si>
+    <t>Associated data file version</t>
+  </si>
+  <si>
+    <t>The version of the dataset (the actual data).</t>
+  </si>
+  <si>
+    <t>Contributor role</t>
+  </si>
+  <si>
+    <t>Type of contribution of the person to the investigation (e.g. data submitter; author; corresponding author)</t>
+  </si>
+  <si>
+    <t>Contributor ID</t>
+  </si>
+  <si>
+    <t>An identifier for the data submitter. If that submitter is an individual, ORCID identifiers are recommended.</t>
   </si>
 </sst>
 </file>
@@ -365,7 +413,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -428,6 +476,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -435,7 +492,7 @@
     <cellStyle name="Normal 4" xfId="1" xr:uid="{AC6FD0CA-C916-4E1F-8927-7A9CF5AB4487}"/>
     <cellStyle name="Warning Text" xfId="3" builtinId="11"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="27">
     <dxf>
       <numFmt numFmtId="164" formatCode="yyyymmdd"/>
     </dxf>
@@ -479,18 +536,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -535,6 +580,56 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -621,8 +716,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="24"/>
-      <tableStyleElement type="headerRow" dxfId="23"/>
+      <tableStyleElement type="wholeTable" dxfId="26"/>
+      <tableStyleElement type="headerRow" dxfId="25"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -637,12 +732,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CDFAA9A6-0123-422D-B80F-81EB2270DAA0}" name="Table7" displayName="Table7" ref="A1:C12" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:C12" xr:uid="{DCA4608A-E2D9-45F1-81E3-F49396F38526}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{1B2189FC-24B3-46E2-BD76-5C288345138F}" name="Table712" displayName="Table712" ref="A1:C18" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:C18" xr:uid="{1B2189FC-24B3-46E2-BD76-5C288345138F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1E03C996-7263-422B-8AA0-13669C78161F}" name="LABEL" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{A20F043F-90CD-41BB-866B-522B95F3EC18}" name="DEFINITION" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{139364FF-5D24-40BF-A84C-CF209A3E5D65}" name="VALUE" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{BABA9F94-FCEF-455B-A517-5C5FE286EF44}" name="LABEL" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{CA68F3E9-F6A1-467D-9AE4-8FE30D2FA8E7}" name="DEFINITION" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{C62A12A3-2BB1-42BC-A1DC-FB6582A6282E}" name="VALUE" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -664,11 +759,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35BDF020-ABCA-4439-B958-8014090B32CC}" name="Table8" displayName="Table8" ref="A1:G2" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:G2" xr:uid="{1B38FBA2-DC2A-4EE8-9782-869C402F129F}"/>
-  <tableColumns count="7">
-    <tableColumn id="2" xr3:uid="{11A585B5-EAF2-4086-9D85-0D60A53887C4}" name="Last Name" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{4077ACA3-84ED-4981-AB4E-365AEBA76825}" name="First Name" dataDxfId="13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35BDF020-ABCA-4439-B958-8014090B32CC}" name="Table8" displayName="Table8" ref="A1:I2" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A1:I2" xr:uid="{1B38FBA2-DC2A-4EE8-9782-869C402F129F}"/>
+  <tableColumns count="9">
+    <tableColumn id="2" xr3:uid="{11A585B5-EAF2-4086-9D85-0D60A53887C4}" name="Last Name" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{4077ACA3-84ED-4981-AB4E-365AEBA76825}" name="First Name" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{FDBF6E14-AF07-43E4-9EDB-2D581CE95920}" name="Contributor role" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{FD848BA4-98DF-42B2-B364-26198B642D3E}" name="Contributor ID" dataDxfId="13"/>
     <tableColumn id="4" xr3:uid="{0A90BD52-57A6-4CDE-BA8E-5136E8A1EAB8}" name="Email" dataDxfId="12"/>
     <tableColumn id="5" xr3:uid="{03F1C9C1-7B2C-4F0C-B099-1F465D301B93}" name="Phone" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{65BCBC93-FC74-4E14-B6A5-BF465AB5D91D}" name="Contributor" dataDxfId="10"/>
@@ -1024,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,51 +1249,107 @@
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="A13" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="30"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-    </row>
-    <row r="15" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A14" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="30"/>
+    </row>
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="30"/>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="30"/>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="30"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="30"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B21" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="12"/>
-    </row>
-    <row r="17" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="14"/>
-    </row>
-    <row r="19" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="12"/>
+    </row>
+    <row r="23" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="14"/>
+    </row>
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B25" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B27" s="18" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="containsBlanks" dxfId="22" priority="1">
+    <cfRule type="containsBlanks" dxfId="24" priority="1">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1260,67 +1413,79 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2115B6D0-8EC1-4029-B8F6-04E7D9736B3A}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" style="22" customWidth="1"/>
-    <col min="3" max="3" width="46.42578125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="53.140625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="25" style="22" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="22" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="22"/>
+    <col min="2" max="4" width="40.85546875" style="22" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="53.140625" style="23" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="25" style="22" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="22" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="F2" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="G2" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="H2" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="I2" s="20" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- CHG: More alignment of templates.
- CHG: Reordering of sheets to move most important sheets to the front.
</commit_message>
<xml_diff>
--- a/chemical-compound-data/compound-data.xlsx
+++ b/chemical-compound-data/compound-data.xlsx
@@ -8,27 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sr41756\workspaces\misc\germinate-data-templates\chemical-compound-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22E486E-4E06-4536-A384-CFD441B7E2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CD8ABB-CFCD-45B7-A2B4-CB3153588621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="3" r:id="rId1"/>
-    <sheet name="LOCATION" sheetId="10" r:id="rId2"/>
-    <sheet name="COLLABORATORS" sheetId="9" r:id="rId3"/>
-    <sheet name="COMPOUNDS" sheetId="2" r:id="rId4"/>
-    <sheet name="DATA" sheetId="6" r:id="rId5"/>
-    <sheet name="RECORDING_DATES" sheetId="7" r:id="rId6"/>
-    <sheet name="COMPOUNDS_EXAMPLE" sheetId="5" r:id="rId7"/>
-    <sheet name="DATA_EXAMPLE" sheetId="4" r:id="rId8"/>
-    <sheet name="RECORDING_DATES_EXAMPLE" sheetId="8" r:id="rId9"/>
+    <sheet name="COMPOUNDS" sheetId="2" r:id="rId2"/>
+    <sheet name="DATA" sheetId="6" r:id="rId3"/>
+    <sheet name="RECORDING_DATES" sheetId="7" r:id="rId4"/>
+    <sheet name="ATTRIBUTES" sheetId="11" r:id="rId5"/>
+    <sheet name="COLLABORATORS" sheetId="9" r:id="rId6"/>
+    <sheet name="LOCATION" sheetId="10" r:id="rId7"/>
+    <sheet name="COMPOUNDS_EXAMPLE" sheetId="5" r:id="rId8"/>
+    <sheet name="DATA_EXAMPLE" sheetId="4" r:id="rId9"/>
+    <sheet name="RECORDING_DATES_EXAMPLE" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -58,9 +59,6 @@
   </si>
   <si>
     <t>Additional Information</t>
-  </si>
-  <si>
-    <t>Please include any additional information that details how this experiment was carried out in a text or Word document and send along with this template. If there are any images please send these as individual JPG files.</t>
   </si>
   <si>
     <t>Help and Assistance</t>
@@ -295,6 +293,30 @@
   </si>
   <si>
     <t>An identifier for the data submitter. If that submitter is an individual, ORCID identifiers are recommended.</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>ValidTypes</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>categorical</t>
+  </si>
+  <si>
+    <t>Please include any additional information that details how this experiment was carried out in a text or Word document and send along with this template. If there are any images please send these as individual JPG files. Mandatory fields are highlighted in yellow.</t>
   </si>
 </sst>
 </file>
@@ -512,20 +534,6 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -590,6 +598,20 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -743,40 +765,20 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{54BDA44A-CD87-4E45-AED3-C04513F7E914}" name="Table9" displayName="Table9" ref="A1:F2" totalsRowShown="0">
-  <autoFilter ref="A1:F2" xr:uid="{F62B6A96-E1F2-40B5-8B32-4E4F94F6494A}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8A8F49BB-5B5C-4DA6-BCFF-0458FF526B9E}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{5863ACB9-3750-47DF-B55F-40C0B119E7E4}" name="Short name"/>
-    <tableColumn id="3" xr3:uid="{C3E73087-AAA0-4C32-A529-1FB205F5DCCE}" name="Country"/>
-    <tableColumn id="4" xr3:uid="{ECF010CE-69C0-49B6-84B9-F22057CDAFB0}" name="Elevation"/>
-    <tableColumn id="5" xr3:uid="{A7D62594-421F-420D-AF72-E3320E9B4E38}" name="Latitude"/>
-    <tableColumn id="6" xr3:uid="{1F86E5D8-33FD-45F7-87AD-13D2B6EDCA41}" name="Longitude"/>
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table44" displayName="Table44" ref="A1:D12" totalsRowShown="0">
+  <autoFilter ref="A1:D12" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Line/Phenotype"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Quercetin" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Catechin" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Epicatechin" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35BDF020-ABCA-4439-B958-8014090B32CC}" name="Table8" displayName="Table8" ref="A1:I2" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A1:I2" xr:uid="{1B38FBA2-DC2A-4EE8-9782-869C402F129F}"/>
-  <tableColumns count="9">
-    <tableColumn id="2" xr3:uid="{11A585B5-EAF2-4086-9D85-0D60A53887C4}" name="Last Name" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{4077ACA3-84ED-4981-AB4E-365AEBA76825}" name="First Name" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{FDBF6E14-AF07-43E4-9EDB-2D581CE95920}" name="Contributor role" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{FD848BA4-98DF-42B2-B364-26198B642D3E}" name="Contributor ID" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{0A90BD52-57A6-4CDE-BA8E-5136E8A1EAB8}" name="Email" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{03F1C9C1-7B2C-4F0C-B099-1F465D301B93}" name="Phone" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{65BCBC93-FC74-4E14-B6A5-BF465AB5D91D}" name="Contributor" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{5C332E95-780E-414E-B1E2-86318BE35F31}" name="Address" dataDxfId="9"/>
-    <tableColumn id="1" xr3:uid="{9A8DCFA6-0AF2-4BA7-95EB-E0D0FE3A6153}" name="Country" dataDxfId="8"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDF6150C-EB7C-4511-B47B-2F8122570053}" name="Table136" displayName="Table136" ref="A1:I2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:I2" xr:uid="{4E670C69-5459-4D42-BBD4-1C0FE57A115B}"/>
   <tableColumns count="9">
@@ -794,7 +796,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{22E566EA-CF41-4BD4-A877-BF1A04CBE27C}" name="Table47" displayName="Table47" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowCellStyle="Warning Text">
   <autoFilter ref="A1:A2" xr:uid="{C24E8378-3794-454E-84CF-B08C2B5A27D2}"/>
   <tableColumns count="1">
@@ -804,7 +806,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E4E9D794-B34F-44CE-84F6-AA0D14CDB5C6}" name="Table4411" displayName="Table4411" ref="A1:A2" totalsRowShown="0">
   <autoFilter ref="A1:A2" xr:uid="{7A5E0959-3CB3-48DB-A1FB-2A58B80F3191}"/>
   <tableColumns count="1">
@@ -814,7 +816,52 @@
 </table>
 </file>
 
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1994A42E-F4CF-4630-8DE3-4A58C976470D}" name="Table14" displayName="Table14" ref="A1:C2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:C2" xr:uid="{1994A42E-F4CF-4630-8DE3-4A58C976470D}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{594B9BB1-1244-4CF5-B4F5-8A80A0DCE1D0}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{2C5F1595-7DD8-4993-8F7E-E8AABDB6D70B}" name="Type"/>
+    <tableColumn id="2" xr3:uid="{97D807EA-7FBC-4355-AAFA-DB4482E6D0CD}" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35BDF020-ABCA-4439-B958-8014090B32CC}" name="Table8" displayName="Table8" ref="A1:I2" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:I2" xr:uid="{1B38FBA2-DC2A-4EE8-9782-869C402F129F}"/>
+  <tableColumns count="9">
+    <tableColumn id="2" xr3:uid="{11A585B5-EAF2-4086-9D85-0D60A53887C4}" name="Last Name" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{4077ACA3-84ED-4981-AB4E-365AEBA76825}" name="First Name" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{FDBF6E14-AF07-43E4-9EDB-2D581CE95920}" name="Contributor role" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{FD848BA4-98DF-42B2-B364-26198B642D3E}" name="Contributor ID" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{0A90BD52-57A6-4CDE-BA8E-5136E8A1EAB8}" name="Email" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{03F1C9C1-7B2C-4F0C-B099-1F465D301B93}" name="Phone" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{65BCBC93-FC74-4E14-B6A5-BF465AB5D91D}" name="Contributor" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{5C332E95-780E-414E-B1E2-86318BE35F31}" name="Address" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{9A8DCFA6-0AF2-4BA7-95EB-E0D0FE3A6153}" name="Country" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{54BDA44A-CD87-4E45-AED3-C04513F7E914}" name="Table9" displayName="Table9" ref="A1:F2" totalsRowShown="0">
+  <autoFilter ref="A1:F2" xr:uid="{F62B6A96-E1F2-40B5-8B32-4E4F94F6494A}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{8A8F49BB-5B5C-4DA6-BCFF-0458FF526B9E}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{5863ACB9-3750-47DF-B55F-40C0B119E7E4}" name="Short name"/>
+    <tableColumn id="3" xr3:uid="{C3E73087-AAA0-4C32-A529-1FB205F5DCCE}" name="Country"/>
+    <tableColumn id="4" xr3:uid="{ECF010CE-69C0-49B6-84B9-F22057CDAFB0}" name="Elevation"/>
+    <tableColumn id="5" xr3:uid="{A7D62594-421F-420D-AF72-E3320E9B4E38}" name="Latitude"/>
+    <tableColumn id="6" xr3:uid="{1F86E5D8-33FD-45F7-87AD-13D2B6EDCA41}" name="Longitude"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{813B0BB4-8EAD-42A9-9C38-FCCCA4584B13}" name="Table1362" displayName="Table1362" ref="A1:I4" totalsRowShown="0">
   <autoFilter ref="A1:I4" xr:uid="{7DC2E6E2-8178-4666-A243-5BBA76D4BFA6}"/>
   <tableColumns count="9">
@@ -832,7 +879,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:D12" totalsRowShown="0">
   <autoFilter ref="A1:D12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
@@ -840,19 +887,6 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Quercetin" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Catechin" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Epicatechin" dataDxfId="3"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table44" displayName="Table44" ref="A1:D12" totalsRowShown="0">
-  <autoFilter ref="A1:D12" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Line/Phenotype"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Quercetin" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Catechin" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Epicatechin" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1140,21 +1174,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="C1" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="8"/>
     </row>
@@ -1163,79 +1197,79 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="19"/>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="8"/>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="C11" s="8"/>
     </row>
@@ -1244,61 +1278,61 @@
         <v>2</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="29" t="s">
         <v>69</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>70</v>
       </c>
       <c r="C13" s="30"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="29" t="s">
         <v>71</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>72</v>
       </c>
       <c r="C14" s="30"/>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="29" t="s">
         <v>73</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>74</v>
       </c>
       <c r="C15" s="30"/>
     </row>
     <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="29" t="s">
         <v>75</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>76</v>
       </c>
       <c r="C16" s="30"/>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="29" t="s">
         <v>77</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>78</v>
       </c>
       <c r="C17" s="30"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="29" t="s">
         <v>79</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>80</v>
       </c>
       <c r="C18" s="30"/>
     </row>
@@ -1317,7 +1351,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1331,20 +1365,20 @@
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1361,47 +1395,385 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C867D861-9536-4856-8988-38BB3B3563D5}">
-  <dimension ref="A1:F1"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="B2" sqref="B2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" t="s">
-        <v>54</v>
-      </c>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4">
+        <v>42371</v>
+      </c>
+      <c r="C2" s="4">
+        <v>42373</v>
+      </c>
+      <c r="D2" s="4">
+        <v>42373</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4">
+        <v>42370</v>
+      </c>
+      <c r="C3" s="4">
+        <v>42375</v>
+      </c>
+      <c r="D3" s="4">
+        <v>42370</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4">
+        <v>42377</v>
+      </c>
+      <c r="C4" s="4">
+        <v>42372</v>
+      </c>
+      <c r="D4" s="4">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4">
+        <v>42378</v>
+      </c>
+      <c r="C5" s="4">
+        <v>42377</v>
+      </c>
+      <c r="D5" s="4">
+        <v>42374</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4">
+        <v>42376</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4">
+        <v>42373</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4">
+        <v>42374</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4">
+        <v>42375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4">
+        <v>42371</v>
+      </c>
+      <c r="C8" s="4">
+        <v>42374</v>
+      </c>
+      <c r="D8" s="4">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4">
+        <v>42379</v>
+      </c>
+      <c r="C9" s="4">
+        <v>42376</v>
+      </c>
+      <c r="D9" s="4">
+        <v>42373</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4">
+        <v>42373</v>
+      </c>
+      <c r="C10" s="4">
+        <v>42374</v>
+      </c>
+      <c r="D10" s="4">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>42379</v>
+      </c>
+      <c r="C11" s="4">
+        <v>42376</v>
+      </c>
+      <c r="D11" s="4">
+        <v>42374</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4">
+        <v>42370</v>
+      </c>
+      <c r="D12" s="4">
+        <v>42372</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="ISO 3166-1 alpha-2" prompt="https://en.wikipedia.org/wiki/ISO_3166-1_alpha-2_x000a_" sqref="C1" xr:uid="{0D9EB899-F3F3-4ABD-A285-8DBAE030C105}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Same format as the &quot;DATA&quot; sheet, but this time the recording date goes into the matrix cells. Dates should be formatted according to the &quot;ACQDATE&quot; field of the MCPD." sqref="A1" xr:uid="{00000000-0002-0000-0600-000000000000}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="20.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="containsBlanks" dxfId="18" priority="1">
+      <formula>LEN(TRIM(A2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phenotype Name" prompt="This should be the full name of the phenotype that has been scored." sqref="A1" xr:uid="{53C12F0B-3F9F-48BF-B0F0-E08B964BA4CC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phenotype Description" prompt="This should be a full description of the phenotype. There is no limit to the length of text that can be used here so please be descriptive." sqref="B1" xr:uid="{F089AE66-013F-4735-81BE-5882571D1849}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Molecular Formula" prompt="The molecular formula of the compound, e.g. C15H14O6" sqref="C1" xr:uid="{A6ED4372-47F5-459B-80DA-BDA21DAD41B6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Name" prompt="The name of the unit that is defined. Examples would include 'centimetre' or 'litre'" sqref="G1" xr:uid="{812908F9-58E0-44B7-8D9B-8F24F8373A14}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Abbreviation" prompt="Abbreviation for unit. Examples include 'l' or 'cm'" sqref="H1" xr:uid="{240F401A-C0EB-48A0-9B93-B4062FF9E866}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Description" prompt="A description of the unit." sqref="I1" xr:uid="{6BD03C10-201D-4FCC-A927-CC3E06375029}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="D1 E1 F1" xr:uid="{FDE2E2F7-197E-4C03-B9BE-2D6744DA16FB}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:A12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="containsBlanks" dxfId="17" priority="1">
+      <formula>LEN(TRIM(A2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Lines (ACCENUMB from MCPD data) on the Y axis and phenotypes (which are described in PHENOTYPES tab) on the x axis. The actual phenotype value goes in the matrix cells. See DATA_EXAMPLE tab for more information before completion." sqref="A1" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1411,7 +1783,102 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+    </row>
+  </sheetData>
+  <dataValidations xWindow="96" yWindow="450" count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Same format as the &quot;DATA&quot; sheet, but this time the recording date goes into the matrix cells. Dates should be formatted according to the &quot;ACQDATE&quot; field of the MCPD." sqref="A1" xr:uid="{13E30841-E8AE-4AEA-9BB5-750247107F69}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D7BB4F-99FF-4A8D-AE3B-39863D7FC541}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F34" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{F3A8F05D-25ED-42E7-993B-6E9C1E5F45A1}">
+      <formula1>$H$2:$H$5</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2115B6D0-8EC1-4029-B8F6-04E7D9736B3A}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -1433,60 +1900,60 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>39</v>
-      </c>
       <c r="C1" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="20" t="s">
-        <v>42</v>
-      </c>
       <c r="I1" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="C2" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="20" t="s">
+      <c r="F2" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="H2" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="20" t="s">
-        <v>48</v>
-      </c>
       <c r="I2" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1498,159 +1965,47 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I4"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C867D861-9536-4856-8988-38BB3B3563D5}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="20.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="containsBlanks" dxfId="7" priority="1">
-      <formula>LEN(TRIM(A2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="7">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phenotype Name" prompt="This should be the full name of the phenotype that has been scored." sqref="A1" xr:uid="{53C12F0B-3F9F-48BF-B0F0-E08B964BA4CC}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phenotype Description" prompt="This should be a full description of the phenotype. There is no limit to the length of text that can be used here so please be descriptive." sqref="B1" xr:uid="{F089AE66-013F-4735-81BE-5882571D1849}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Molecular Formula" prompt="The molecular formula of the compound, e.g. C15H14O6" sqref="C1" xr:uid="{A6ED4372-47F5-459B-80DA-BDA21DAD41B6}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Name" prompt="The name of the unit that is defined. Examples would include 'centimetre' or 'litre'" sqref="G1" xr:uid="{812908F9-58E0-44B7-8D9B-8F24F8373A14}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Abbreviation" prompt="Abbreviation for unit. Examples include 'l' or 'cm'" sqref="H1" xr:uid="{240F401A-C0EB-48A0-9B93-B4062FF9E866}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Description" prompt="A description of the unit." sqref="I1" xr:uid="{6BD03C10-201D-4FCC-A927-CC3E06375029}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="D1 E1 F1" xr:uid="{FDE2E2F7-197E-4C03-B9BE-2D6744DA16FB}"/>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="containsBlanks" dxfId="6" priority="1">
-      <formula>LEN(TRIM(A2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Lines (ACCENUMB from MCPD data) on the Y axis and phenotypes (which are described in PHENOTYPES tab) on the x axis. The actual phenotype value goes in the matrix cells. See DATA_EXAMPLE tab for more information before completion." sqref="A1" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="ISO 3166-1 alpha-2" prompt="https://en.wikipedia.org/wiki/ISO_3166-1_alpha-2_x000a_" sqref="C1" xr:uid="{0D9EB899-F3F3-4ABD-A285-8DBAE030C105}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1660,39 +2015,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-    </row>
-  </sheetData>
-  <dataValidations xWindow="96" yWindow="450" count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Same format as the &quot;DATA&quot; sheet, but this time the recording date goes into the matrix cells. Dates should be formatted according to the &quot;ACQDATE&quot; field of the MCPD." sqref="A1" xr:uid="{13E30841-E8AE-4AEA-9BB5-750247107F69}"/>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -1724,16 +2047,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>8</v>
@@ -1747,11 +2070,11 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2" s="3">
         <v>302.042664</v>
@@ -1760,7 +2083,7 @@
         <v>302.23599999999999</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -1768,10 +2091,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
         <v>64</v>
-      </c>
-      <c r="C3" t="s">
-        <v>65</v>
       </c>
       <c r="D3">
         <v>290.07904100000002</v>
@@ -1780,15 +2103,15 @@
         <v>290.26799999999997</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4">
         <v>290.07904100000002</v>
@@ -1797,7 +2120,7 @@
         <v>290.26799999999997</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1817,7 +2140,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -1841,18 +2164,18 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>1430.92</v>
@@ -1866,7 +2189,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>9545.9</v>
@@ -1880,7 +2203,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>4409.87</v>
@@ -1894,7 +2217,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>7877.64</v>
@@ -1908,7 +2231,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>8413.19</v>
@@ -1919,7 +2242,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>4811.21</v>
@@ -1930,7 +2253,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>2961.11</v>
@@ -1944,7 +2267,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>5358.59</v>
@@ -1958,7 +2281,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>6235.09</v>
@@ -1972,7 +2295,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>6945.25</v>
@@ -1986,7 +2309,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>5249.35</v>
@@ -2002,230 +2325,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
-    <tabColor theme="4"/>
-  </sheetPr>
-  <dimension ref="A1:D20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="4">
-        <v>42371</v>
-      </c>
-      <c r="C2" s="4">
-        <v>42373</v>
-      </c>
-      <c r="D2" s="4">
-        <v>42373</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="4">
-        <v>42370</v>
-      </c>
-      <c r="C3" s="4">
-        <v>42375</v>
-      </c>
-      <c r="D3" s="4">
-        <v>42370</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="4">
-        <v>42377</v>
-      </c>
-      <c r="C4" s="4">
-        <v>42372</v>
-      </c>
-      <c r="D4" s="4">
-        <v>42377</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="4">
-        <v>42378</v>
-      </c>
-      <c r="C5" s="4">
-        <v>42377</v>
-      </c>
-      <c r="D5" s="4">
-        <v>42374</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="4">
-        <v>42376</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4">
-        <v>42373</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="4">
-        <v>42374</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4">
-        <v>42375</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4">
-        <v>42371</v>
-      </c>
-      <c r="C8" s="4">
-        <v>42374</v>
-      </c>
-      <c r="D8" s="4">
-        <v>42376</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="4">
-        <v>42379</v>
-      </c>
-      <c r="C9" s="4">
-        <v>42376</v>
-      </c>
-      <c r="D9" s="4">
-        <v>42373</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="4">
-        <v>42373</v>
-      </c>
-      <c r="C10" s="4">
-        <v>42374</v>
-      </c>
-      <c r="D10" s="4">
-        <v>42376</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="4">
-        <v>42379</v>
-      </c>
-      <c r="C11" s="4">
-        <v>42376</v>
-      </c>
-      <c r="D11" s="4">
-        <v>42374</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4">
-        <v>42370</v>
-      </c>
-      <c r="D12" s="4">
-        <v>42372</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="4"/>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Same format as the &quot;DATA&quot; sheet, but this time the recording date goes into the matrix cells. Dates should be formatted according to the &quot;ACQDATE&quot; field of the MCPD." sqref="A1" xr:uid="{00000000-0002-0000-0600-000000000000}"/>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>